<commit_message>
hoàn thiện các chức năng còn lại
</commit_message>
<xml_diff>
--- a/asm_DangKi/bin/Debug/DoanhThu.xlsx
+++ b/asm_DangKi/bin/Debug/DoanhThu.xlsx
@@ -41,16 +41,16 @@
     <t xml:space="preserve">DT001</t>
   </si>
   <si>
-    <t xml:space="preserve">31/07/2023 12:00:00 AM</t>
+    <t xml:space="preserve">04/08/2023 12:00:00 AM</t>
   </si>
   <si>
-    <t xml:space="preserve">145000</t>
+    <t xml:space="preserve">15000</t>
   </si>
   <si>
     <t xml:space="preserve">kien001</t>
   </si>
   <si>
-    <t xml:space="preserve">2</t>
+    <t xml:space="preserve">1</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
Hoàn thiện và fix một số lỗi cơ bản
</commit_message>
<xml_diff>
--- a/asm_DangKi/bin/Debug/DoanhThu.xlsx
+++ b/asm_DangKi/bin/Debug/DoanhThu.xlsx
@@ -35,7 +35,7 @@
     <t xml:space="preserve">MaHoaDon1</t>
   </si>
   <si>
-    <t xml:space="preserve">HD001</t>
+    <t xml:space="preserve">HD003</t>
   </si>
   <si>
     <t xml:space="preserve">DT001</t>
@@ -44,7 +44,7 @@
     <t xml:space="preserve">04/08/2023 12:00:00 AM</t>
   </si>
   <si>
-    <t xml:space="preserve">15000</t>
+    <t xml:space="preserve">36000</t>
   </si>
   <si>
     <t xml:space="preserve">kien001</t>

</xml_diff>